<commit_message>
modifs rapport4 + change name of tache2
</commit_message>
<xml_diff>
--- a/rapport4/HAZOP.xlsx
+++ b/rapport4/HAZOP.xlsx
@@ -1,30 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnaud\Desktop\projet-1225\rapport4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Causes</t>
   </si>
@@ -115,12 +113,22 @@
 Explosion du réacteur.
 </t>
   </si>
+  <si>
+    <t>Blackout électrique</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Réacteur surchauffe. Arrêt de la réaction et redémarrage nécessaire</t>
+  </si>
+  <si>
+    <t>Générateurs de sécurité sur le site. Disques de rupture au niveau du réacteur.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +151,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,6 +180,9 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -175,9 +190,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -191,7 +203,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -246,7 +258,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +293,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,55 +470,55 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" ht="90" customHeight="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" ht="90" customHeight="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -519,67 +531,78 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" ht="90" customHeight="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3">
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3">
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3">
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3">
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3">
       <c r="C21" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>